<commit_message>
Test 1 Complete And Successfull
</commit_message>
<xml_diff>
--- a/Tipos.xlsx
+++ b/Tipos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,30 +441,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Domingo</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Jueves</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Lunes</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Martes</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Miercoles</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Sabado</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Viernes</t>
         </is>
@@ -480,6 +485,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -493,6 +499,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -506,6 +513,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -519,6 +527,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -532,6 +541,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -545,6 +555,7 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -558,6 +569,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -571,6 +583,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -584,6 +597,7 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -597,6 +611,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -610,6 +625,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -623,6 +639,7 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -636,6 +653,7 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -649,6 +667,7 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -662,6 +681,7 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -675,6 +695,7 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -688,6 +709,7 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -701,6 +723,7 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -714,6 +737,7 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -727,6 +751,7 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -740,6 +765,7 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -753,6 +779,7 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -766,6 +793,7 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -779,6 +807,7 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -792,6 +821,7 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -805,6 +835,7 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -818,6 +849,7 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -831,6 +863,7 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -844,6 +877,7 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -857,6 +891,7 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -870,6 +905,7 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -883,6 +919,7 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -896,6 +933,7 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -909,6 +947,7 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -922,6 +961,7 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -935,6 +975,7 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -948,6 +989,7 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -961,6 +1003,7 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -974,6 +1017,7 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -987,6 +1031,7 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -1000,6 +1045,7 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -1013,6 +1059,7 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -1026,6 +1073,7 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -1039,6 +1087,7 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -1052,6 +1101,7 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -1065,6 +1115,7 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -1078,6 +1129,7 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -1091,6 +1143,7 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -1104,6 +1157,7 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1117,6 +1171,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -1130,6 +1185,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -1143,6 +1199,7 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -1156,6 +1213,7 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -1169,6 +1227,7 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>